<commit_message>
Minor changes to graph
</commit_message>
<xml_diff>
--- a/Graphs.xlsx
+++ b/Graphs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paanir/Dropbox/Study/3.DS/Proj2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paanir/Distributed-Systems-Projects/project2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -54,9 +54,6 @@
     <t>Convergence = All nodes have heard the rumor at least once</t>
   </si>
   <si>
-    <t>Convergence = 75 % of nodes have converged to some value</t>
-  </si>
-  <si>
     <t>line (50%)</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>Convergence times for Push-Sum (in :native time units)</t>
+  </si>
+  <si>
+    <t>Convergence = 75 % of nodes have converged to some value (50% for line topology)</t>
   </si>
 </sst>
 </file>
@@ -801,11 +801,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1903429728"/>
-        <c:axId val="1903434000"/>
+        <c:axId val="1913833600"/>
+        <c:axId val="1913837232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1903429728"/>
+        <c:axId val="1913833600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -928,12 +928,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1903434000"/>
+        <c:crossAx val="1913837232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1903434000"/>
+        <c:axId val="1913837232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1013,6 +1013,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1049,7 +1050,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1903429728"/>
+        <c:crossAx val="1913833600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1764,11 +1765,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1903474112"/>
-        <c:axId val="1903478384"/>
+        <c:axId val="1913949424"/>
+        <c:axId val="1913953056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1903474112"/>
+        <c:axId val="1913949424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1880,12 +1881,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1903478384"/>
+        <c:crossAx val="1913953056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1903478384"/>
+        <c:axId val="1913953056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1997,7 +1998,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1903474112"/>
+        <c:crossAx val="1913949424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2620,11 +2621,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1903509520"/>
-        <c:axId val="1903513792"/>
+        <c:axId val="1915600912"/>
+        <c:axId val="1915603856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1903509520"/>
+        <c:axId val="1915600912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2740,12 +2741,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1903513792"/>
+        <c:crossAx val="1915603856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1903513792"/>
+        <c:axId val="1915603856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2857,7 +2858,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1903509520"/>
+        <c:crossAx val="1915600912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4979,8 +4980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="B63" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4997,7 +4998,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -5331,7 +5332,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -5646,12 +5647,12 @@
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B64" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B65" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -5662,7 +5663,7 @@
         <v>1</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>3</v>
@@ -5704,7 +5705,7 @@
         <v>203249000</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E68" s="3">
         <v>818390000</v>
@@ -5725,7 +5726,7 @@
         <v>820825000</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E69" s="3">
         <v>1244022000</v>

</xml_diff>

<commit_message>
Made few changes. Remade graphs
</commit_message>
<xml_diff>
--- a/Graphs.xlsx
+++ b/Graphs.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="14">
   <si>
     <t>num_nodes</t>
   </si>
@@ -57,22 +57,19 @@
     <t>line (50%)</t>
   </si>
   <si>
-    <t>or converge very slowly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do not converge </t>
-  </si>
-  <si>
-    <t>Convergence times for Gossip (in :native time units)</t>
-  </si>
-  <si>
-    <t>Convergence times for Push-Sum (in :native time units)</t>
-  </si>
-  <si>
     <t>Convergence = 75 % of nodes have converged to some value (50% for line topology)</t>
   </si>
   <si>
-    <t>Consider it to be the x-axis</t>
+    <t>Consider it to be the y-axis</t>
+  </si>
+  <si>
+    <t>Convergence times for Gossip (in microseconds)</t>
+  </si>
+  <si>
+    <t>Convergence times for Push-Sum (in microseconds)</t>
+  </si>
+  <si>
+    <t>Converge very slowly</t>
   </si>
 </sst>
 </file>
@@ -143,13 +140,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -270,9 +266,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0434162015614148"/>
-          <c:y val="0.0126068263433598"/>
-          <c:w val="0.931780715709769"/>
+          <c:x val="0.0664000878645534"/>
+          <c:y val="0.0192302298090601"/>
+          <c:w val="0.91139442735967"/>
           <c:h val="0.85687642078213"/>
         </c:manualLayout>
       </c:layout>
@@ -312,57 +308,6 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>29000.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0052E8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.01796E8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.0274E8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.04735E8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.05365E8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.07572E8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.08655E8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.00991E9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8.28229E8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.840938E9</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.183075E9</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5.632767E9</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8.7374755E10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
               <c:f>Sheet1!$A$4:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -411,126 +356,54 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Line</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="6"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$4:$C$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>32000.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.01319E8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.02801E8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.019704772E9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.62548173E9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.859851862E9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.074803663E9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.394586919E10</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.2687765752E10</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.1992044514E10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.63495081E11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.2037515E11</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$15</c:f>
+              <c:f>Sheet1!$B$4:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>41.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0</c:v>
+                  <c:v>2880.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0</c:v>
+                  <c:v>105259.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.0</c:v>
+                  <c:v>206177.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.0</c:v>
+                  <c:v>206843.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>64.0</c:v>
+                  <c:v>105919.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>128.0</c:v>
+                  <c:v>207147.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>256.0</c:v>
+                  <c:v>207222.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>512.0</c:v>
+                  <c:v>209141.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1024.0</c:v>
+                  <c:v>211556.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2048.0</c:v>
+                  <c:v>246896.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4096.0</c:v>
+                  <c:v>330475.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.008441E6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.724843E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -539,7 +412,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>2D</c:v>
           </c:tx>
@@ -570,57 +443,6 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$4:$D$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>2.04193E8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.08779E8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.04283E8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.0729E8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8.0796E8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.415432E9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.224206E9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.720043E9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.136964E9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.151101E9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6.173119E9</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5.78044E9</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.2741358E10</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.27677E10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
               <c:f>Sheet1!$F$4:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -666,6 +488,57 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>34969.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>105464.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>206380.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>509158.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>306823.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>510164.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.015731E6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.524126E6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.625265E6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.736669E6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.139273E6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.657828E6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.193474E6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.940366E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -674,7 +547,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>imp2D</c:v>
           </c:tx>
@@ -688,10 +561,12 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="x"/>
+            <c:symbol val="triangle"/>
             <c:size val="6"/>
             <c:spPr>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent4"/>
@@ -703,57 +578,6 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$4:$E$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>2.03562E8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.02392E8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.03092E8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.009545E9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8.07382E8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.0757E8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.116472E9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.117737E9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.212549E9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.729237E9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.444538E9</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.93465E9</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.841662E9</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2.78456E9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
               <c:f>Sheet1!$F$4:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -799,6 +623,180 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>34969.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$4:$E$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>2215.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>105569.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2285.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>105973.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>105410.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>308061.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>410390.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>517657.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>515451.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>517401.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>520639.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>615677.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>617826.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>733386.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Line</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$4:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2015.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>508345.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>509896.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.222283E6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.418383E6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.935963E6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.000377E6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1526801E7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.6075364E7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.1014327E7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.47796295E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -813,11 +811,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1913833600"/>
-        <c:axId val="1913837232"/>
+        <c:axId val="-1054790192"/>
+        <c:axId val="-1054785648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1913833600"/>
+        <c:axId val="-1054790192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -858,18 +856,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Times</a:t>
+                  <a:t>Number of nodes in topology</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> in Erlang Native units</a:t>
-                </a:r>
-              </a:p>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -940,12 +928,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1913837232"/>
+        <c:crossAx val="-1054785648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1913837232"/>
+        <c:axId val="-1054785648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -986,12 +974,9 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Number</a:t>
+                  <a:t>Times in microseconds</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> of ndoes in topology</a:t>
-                </a:r>
+                <a:endParaRPr lang="en-US" baseline="0"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1062,7 +1047,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1913833600"/>
+        <c:crossAx val="-1054790192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1082,7 +1067,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.837948717948718"/>
           <c:y val="0.182593648074325"/>
-          <c:w val="0.063945267958951"/>
+          <c:w val="0.0601716738197425"/>
           <c:h val="0.192113161427341"/>
         </c:manualLayout>
       </c:layout>
@@ -1186,7 +1171,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="0" cap="all" baseline="0">
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" cap="all" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>Graph-2</a:t>
@@ -1197,12 +1182,12 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="0" cap="all" baseline="0">
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" cap="all" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>Convergence times for gossip </a:t>
             </a:r>
-            <a:endParaRPr lang="en-US">
+            <a:endParaRPr lang="en-US" sz="1400">
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
@@ -1211,12 +1196,12 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="0" cap="all" baseline="0">
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" cap="all" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>(where convergence means 50% of nodes have heard the rumor 10 times)</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US">
+            <a:endParaRPr lang="en-US" sz="1400">
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
@@ -1300,57 +1285,6 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$35:$B$48</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>8.10723E8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.009625E9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.07721E8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.009673E9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8.07662E8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.07806E8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9.09152E8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.09613E8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.10919E8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.14669E8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9.88585E8</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>9.14418E8</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.169282E9</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.1489207E10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
               <c:f>Sheet1!$A$35:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1396,6 +1330,57 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>16384.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$35:$B$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>812258.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.013991E6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.116124E6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.015131E6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.216623E6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.318784E6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.317056E6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.219718E6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.318889E6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.32374E6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.356027E6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.369963E6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.781902E6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.9863209E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1434,84 +1419,93 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>Sheet1!$A$35:$A$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16384.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Sheet1!$C$35:$C$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>8.09959E8</c:v>
+                  <c:v>813138.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.06349E8</c:v>
+                  <c:v>812748.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.111062E9</c:v>
+                  <c:v>913472.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.01975E9</c:v>
+                  <c:v>1.621754E6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.517671E9</c:v>
+                  <c:v>2.327589E6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.956739E9</c:v>
+                  <c:v>2.026578E6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.827292E9</c:v>
+                  <c:v>9.196144E6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.760756E9</c:v>
+                  <c:v>9.398393E6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0823778E10</c:v>
+                  <c:v>2.1228694E7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.81682E10</c:v>
+                  <c:v>6.1829437E7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.2811757743E10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$35:$A$45</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>256.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1024.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2048.0</c:v>
+                  <c:v>1.27336866E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1550,54 +1544,6 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$35:$D$47</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>8.10064E8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.211617E9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.010164E9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.424907E9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.322595E9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.231921E9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.93896E9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.382927E9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.3138433E10</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.484898E10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.8093805E10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.45792731E11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.90431819E11</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
               <c:f>Sheet1!$F$35:$F$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1640,6 +1586,54 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>17424.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$35:$D$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.014623E6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.215642E6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.114906E6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.318345E6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.724848E6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.924899E6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.127092E6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.735827E6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.44122E6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.839096E6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.24807E6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.402775E6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.615509E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1678,57 +1672,6 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$35:$E$48</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>9.11045E8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.212164E9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.01025E9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.122505E9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.110726E9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.010873E9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.212574E9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.319543E9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.314747E9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.321649E9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.21842E9</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.331453E9</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.42704E9</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.458768E9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
               <c:f>Sheet1!$F$35:$F$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1774,6 +1717,57 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>34969.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$35:$E$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1.216458E6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.317671E6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.014318E6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.420024E6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.328238E6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.423336E6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.429144E6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.524594E6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.727115E6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.83225E6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.870407E6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.729132E6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.883162E6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.974957E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1788,11 +1782,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1913949424"/>
-        <c:axId val="1913953056"/>
+        <c:axId val="-1054754752"/>
+        <c:axId val="-1054750480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1913949424"/>
+        <c:axId val="-1054754752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1832,9 +1826,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Times in Erlang Native Units</a:t>
+                  <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Number of nodes in topology</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-US" sz="1200">
+                  <a:effectLst/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1904,12 +1903,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1913953056"/>
+        <c:crossAx val="-1054750480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1913953056"/>
+        <c:axId val="-1054750480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1950,8 +1949,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Number of noes in topology</a:t>
+                  <a:t>Times</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> in microseconds</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2021,7 +2025,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1913949424"/>
+        <c:crossAx val="-1054754752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2243,51 +2247,6 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$68:$B$79</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>3.05209E8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.05576E8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.12705E8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.19475E8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.53616E8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8.89608E8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.014064E9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.244979E9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.761898E9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.423181E9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.2085779E10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6.2770179E10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
               <c:f>Sheet1!$A$68:$A$79</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -2327,6 +2286,51 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$68:$B$79</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>507057.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>507972.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512343.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.425194E6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.139205E6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.089458E6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.514786E6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.01787E6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.462571E6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.940121E6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.6119075E7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.9764083E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2365,57 +2369,6 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$67:$C$80</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>722000.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.03249E8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.20825E8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.024733E9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.926346E9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.872559E9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.496309E9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.840595E9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.301601E9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.887163E9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7.266657E9</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.0008529E10</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.5759075E10</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2.7411723E10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
               <c:f>Sheet1!$A$67:$A$80</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -2464,59 +2417,51 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>2D</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$D$67</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1.03183E8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$67</c:f>
+              <c:f>Sheet1!$C$67:$C$79</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>777.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>203687.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>205375.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>510074.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>317462.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>433415.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>691443.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>808164.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.068686E6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.641384E6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.982439E6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.8976081E7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.5690642E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2525,7 +2470,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>imp2D</c:v>
           </c:tx>
@@ -2555,51 +2500,6 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$67:$E$78</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>1.519057E9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.1839E8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.244022E9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.392942E9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.086793E9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.890661E9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.470549E9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6.261039E9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7.489979E9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.205334E9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.1032582E10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4.6976933E10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
               <c:f>Sheet1!$F$67:$F$78</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -2639,6 +2539,51 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>8649.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$67:$E$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>508680.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.114825E6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.133553E6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.566066E6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.577064E6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.003734E6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.823738E6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.62098E6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.556942E6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.617073E6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0408258E7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.4651993E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2653,11 +2598,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1915600912"/>
-        <c:axId val="1915603856"/>
+        <c:axId val="-1054718688"/>
+        <c:axId val="-1054714928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1915600912"/>
+        <c:axId val="-1054718688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2697,13 +2642,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Times in Erlang Native</a:t>
+                  <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Number of nodes in topology</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Units</a:t>
-                </a:r>
+                <a:endParaRPr lang="en-US" sz="1200">
+                  <a:effectLst/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2773,12 +2719,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1915603856"/>
+        <c:crossAx val="-1054714928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1915603856"/>
+        <c:axId val="-1054714928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2819,8 +2765,14 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Number of nodes in topology</a:t>
+                  <a:t>Times in microseconds</a:t>
                 </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2890,7 +2842,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1915600912"/>
+        <c:crossAx val="-1054718688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2908,8 +2860,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.781379310344828"/>
-          <c:y val="0.161343927962007"/>
+          <c:x val="0.814630541871921"/>
+          <c:y val="0.158732961904566"/>
           <c:w val="0.133645320197044"/>
           <c:h val="0.197129170864086"/>
         </c:manualLayout>
@@ -4662,8 +4614,8 @@
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -5012,8 +4964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C59" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5063,16 +5015,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>29000</v>
+        <v>41</v>
       </c>
       <c r="C4" s="2">
-        <v>32000</v>
+        <v>24</v>
       </c>
       <c r="D4" s="3">
-        <v>204193000</v>
+        <v>2000</v>
       </c>
       <c r="E4" s="3">
-        <v>203562000</v>
+        <v>2215</v>
       </c>
       <c r="F4" s="3">
         <v>4</v>
@@ -5084,16 +5036,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>100520000</v>
+        <v>2880</v>
       </c>
       <c r="C5" s="2">
-        <v>201319000</v>
+        <v>2015</v>
       </c>
       <c r="D5" s="3">
-        <v>908779000</v>
+        <v>105464</v>
       </c>
       <c r="E5" s="3">
-        <v>202392000</v>
+        <v>105569</v>
       </c>
       <c r="F5" s="3">
         <v>9</v>
@@ -5105,16 +5057,16 @@
         <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>201796000</v>
+        <v>105259</v>
       </c>
       <c r="C6" s="2">
-        <v>302801000</v>
+        <v>508345</v>
       </c>
       <c r="D6" s="3">
-        <v>404283000</v>
+        <v>206380</v>
       </c>
       <c r="E6" s="3">
-        <v>303092000</v>
+        <v>2285</v>
       </c>
       <c r="F6" s="3">
         <v>16</v>
@@ -5126,16 +5078,16 @@
         <v>16</v>
       </c>
       <c r="B7" s="2">
-        <v>302740000</v>
+        <v>206177</v>
       </c>
       <c r="C7" s="2">
-        <v>2019704772</v>
+        <v>509896</v>
       </c>
       <c r="D7" s="3">
-        <v>707290000</v>
+        <v>509158</v>
       </c>
       <c r="E7" s="3">
-        <v>1009545000</v>
+        <v>105973</v>
       </c>
       <c r="F7" s="3">
         <v>36</v>
@@ -5147,16 +5099,16 @@
         <v>32</v>
       </c>
       <c r="B8" s="2">
-        <v>504735000</v>
+        <v>206843</v>
       </c>
       <c r="C8" s="2">
-        <v>2625481730</v>
+        <v>1222283</v>
       </c>
       <c r="D8" s="3">
-        <v>807960000</v>
+        <v>306823</v>
       </c>
       <c r="E8" s="3">
-        <v>807382000</v>
+        <v>105410</v>
       </c>
       <c r="F8" s="3">
         <v>64</v>
@@ -5168,16 +5120,16 @@
         <v>64</v>
       </c>
       <c r="B9" s="2">
-        <v>505365000</v>
+        <v>105919</v>
       </c>
       <c r="C9" s="2">
-        <v>5859851862</v>
+        <v>1418383</v>
       </c>
       <c r="D9" s="3">
-        <v>1415432000</v>
+        <v>510164</v>
       </c>
       <c r="E9" s="3">
-        <v>607570000</v>
+        <v>308061</v>
       </c>
       <c r="F9" s="3">
         <v>121</v>
@@ -5189,16 +5141,16 @@
         <v>128</v>
       </c>
       <c r="B10" s="2">
-        <v>707572000</v>
+        <v>207147</v>
       </c>
       <c r="C10" s="2">
-        <v>7074803663</v>
+        <v>2935963</v>
       </c>
       <c r="D10" s="3">
-        <v>2224206000</v>
+        <v>1015731</v>
       </c>
       <c r="E10" s="3">
-        <v>1116472000</v>
+        <v>410390</v>
       </c>
       <c r="F10" s="3">
         <v>256</v>
@@ -5210,16 +5162,16 @@
         <v>256</v>
       </c>
       <c r="B11" s="2">
-        <v>808655000</v>
+        <v>207222</v>
       </c>
       <c r="C11" s="2">
-        <v>13945869190</v>
+        <v>9000377</v>
       </c>
       <c r="D11" s="3">
-        <v>1720043000</v>
+        <v>1524126</v>
       </c>
       <c r="E11" s="3">
-        <v>1117737000</v>
+        <v>517657</v>
       </c>
       <c r="F11" s="3">
         <v>529</v>
@@ -5231,16 +5183,16 @@
         <v>512</v>
       </c>
       <c r="B12" s="2">
-        <v>1009910000</v>
+        <v>209141</v>
       </c>
       <c r="C12" s="2">
-        <v>52687765752</v>
+        <v>11526801</v>
       </c>
       <c r="D12" s="3">
-        <v>3136964000</v>
+        <v>1625265</v>
       </c>
       <c r="E12" s="3">
-        <v>1212549000</v>
+        <v>515451</v>
       </c>
       <c r="F12" s="3">
         <v>1089</v>
@@ -5252,16 +5204,16 @@
         <v>1024</v>
       </c>
       <c r="B13" s="2">
-        <v>828229000</v>
+        <v>211556</v>
       </c>
       <c r="C13" s="2">
-        <v>91992044514</v>
+        <v>26075364</v>
       </c>
       <c r="D13" s="3">
-        <v>4151101000</v>
+        <v>2736669</v>
       </c>
       <c r="E13" s="3">
-        <v>1729237000</v>
+        <v>517401</v>
       </c>
       <c r="F13" s="3">
         <v>2209</v>
@@ -5273,16 +5225,16 @@
         <v>2048</v>
       </c>
       <c r="B14" s="2">
-        <v>1840938000</v>
+        <v>246896</v>
       </c>
       <c r="C14" s="2">
-        <v>163495081000</v>
+        <v>81014327</v>
       </c>
       <c r="D14" s="3">
-        <v>6173119000</v>
+        <v>2139273</v>
       </c>
       <c r="E14" s="3">
-        <v>1444538000</v>
+        <v>520639</v>
       </c>
       <c r="F14" s="3">
         <v>4356</v>
@@ -5294,16 +5246,16 @@
         <v>4096</v>
       </c>
       <c r="B15" s="2">
-        <v>1183075000</v>
+        <v>330475</v>
       </c>
       <c r="C15" s="2">
-        <v>320375150000</v>
+        <v>147796295</v>
       </c>
       <c r="D15" s="3">
-        <v>5780440000</v>
+        <v>3657828</v>
       </c>
       <c r="E15" s="3">
-        <v>2934650000</v>
+        <v>615677</v>
       </c>
       <c r="F15" s="3">
         <v>8649</v>
@@ -5315,16 +5267,16 @@
         <v>8192</v>
       </c>
       <c r="B16" s="2">
-        <v>5632767000</v>
+        <v>1008441</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="3">
-        <v>12741358000</v>
+        <v>5193474</v>
       </c>
       <c r="E16" s="3">
-        <v>1841662000</v>
+        <v>617826</v>
       </c>
       <c r="F16" s="3">
         <v>17424</v>
@@ -5336,16 +5288,16 @@
         <v>16384</v>
       </c>
       <c r="B17" s="2">
-        <v>87374755000</v>
+        <v>7724843</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="3">
-        <v>12767700000</v>
+        <v>7940366</v>
       </c>
       <c r="E17" s="3">
-        <v>2784560000</v>
+        <v>733386</v>
       </c>
       <c r="F17" s="3">
         <v>34969</v>
@@ -5397,16 +5349,16 @@
         <v>2</v>
       </c>
       <c r="B35" s="4">
-        <v>810723000</v>
+        <v>812258</v>
       </c>
       <c r="C35" s="4">
-        <v>809959000</v>
+        <v>813138</v>
       </c>
       <c r="D35" s="3">
-        <v>810064000</v>
+        <v>1014623</v>
       </c>
       <c r="E35" s="3">
-        <v>911045000</v>
+        <v>1216458</v>
       </c>
       <c r="F35" s="3">
         <v>4</v>
@@ -5418,16 +5370,16 @@
         <v>4</v>
       </c>
       <c r="B36" s="4">
-        <v>1009625000</v>
+        <v>1013991</v>
       </c>
       <c r="C36" s="4">
-        <v>606349000</v>
+        <v>812748</v>
       </c>
       <c r="D36" s="3">
-        <v>1211617000</v>
+        <v>1215642</v>
       </c>
       <c r="E36" s="3">
-        <v>1212164000</v>
+        <v>1317671</v>
       </c>
       <c r="F36" s="3">
         <v>9</v>
@@ -5439,16 +5391,16 @@
         <v>8</v>
       </c>
       <c r="B37" s="4">
-        <v>807721000</v>
+        <v>1116124</v>
       </c>
       <c r="C37" s="4">
-        <v>1111062000</v>
+        <v>913472</v>
       </c>
       <c r="D37" s="3">
-        <v>1010164000</v>
+        <v>1114906</v>
       </c>
       <c r="E37" s="3">
-        <v>1010250000</v>
+        <v>1014318</v>
       </c>
       <c r="F37" s="3">
         <v>16</v>
@@ -5460,16 +5412,16 @@
         <v>16</v>
       </c>
       <c r="B38" s="4">
-        <v>1009673000</v>
+        <v>1015131</v>
       </c>
       <c r="C38" s="4">
-        <v>2019750000</v>
+        <v>1621754</v>
       </c>
       <c r="D38" s="3">
-        <v>2424907000</v>
+        <v>1318345</v>
       </c>
       <c r="E38" s="3">
-        <v>1122505000</v>
+        <v>1420024</v>
       </c>
       <c r="F38" s="3">
         <v>36</v>
@@ -5481,16 +5433,16 @@
         <v>32</v>
       </c>
       <c r="B39" s="4">
-        <v>807662000</v>
+        <v>1216623</v>
       </c>
       <c r="C39" s="4">
-        <v>1517671000</v>
+        <v>2327589</v>
       </c>
       <c r="D39" s="3">
-        <v>2322595000</v>
+        <v>1724848</v>
       </c>
       <c r="E39" s="3">
-        <v>1110726000</v>
+        <v>1328238</v>
       </c>
       <c r="F39" s="3">
         <v>64</v>
@@ -5502,16 +5454,16 @@
         <v>64</v>
       </c>
       <c r="B40" s="4">
-        <v>907806000</v>
+        <v>1318784</v>
       </c>
       <c r="C40" s="4">
-        <v>4956739000</v>
+        <v>2026578</v>
       </c>
       <c r="D40" s="3">
-        <v>3231921000</v>
+        <v>1924899</v>
       </c>
       <c r="E40" s="3">
-        <v>1010873000</v>
+        <v>1423336</v>
       </c>
       <c r="F40" s="3">
         <v>121</v>
@@ -5523,16 +5475,16 @@
         <v>128</v>
       </c>
       <c r="B41" s="4">
-        <v>909152000</v>
+        <v>1317056</v>
       </c>
       <c r="C41" s="4">
-        <v>2827292000</v>
+        <v>9196144</v>
       </c>
       <c r="D41" s="3">
-        <v>3938960000</v>
+        <v>2127092</v>
       </c>
       <c r="E41" s="3">
-        <v>1212574000</v>
+        <v>1429144</v>
       </c>
       <c r="F41" s="3">
         <v>256</v>
@@ -5544,16 +5496,16 @@
         <v>256</v>
       </c>
       <c r="B42" s="4">
-        <v>909613000</v>
+        <v>1219718</v>
       </c>
       <c r="C42" s="4">
-        <v>4760756000</v>
+        <v>9398393</v>
       </c>
       <c r="D42" s="3">
-        <v>8382927000</v>
+        <v>2735827</v>
       </c>
       <c r="E42" s="3">
-        <v>1319543000</v>
+        <v>1524594</v>
       </c>
       <c r="F42" s="3">
         <v>529</v>
@@ -5565,16 +5517,16 @@
         <v>512</v>
       </c>
       <c r="B43" s="4">
-        <v>910919000</v>
+        <v>1318889</v>
       </c>
       <c r="C43" s="4">
-        <v>10823778000</v>
+        <v>21228694</v>
       </c>
       <c r="D43" s="3">
-        <v>13138433000</v>
+        <v>2441220</v>
       </c>
       <c r="E43" s="3">
-        <v>1314747000</v>
+        <v>1727115</v>
       </c>
       <c r="F43" s="3">
         <v>1089</v>
@@ -5586,16 +5538,16 @@
         <v>1024</v>
       </c>
       <c r="B44" s="4">
-        <v>914669000</v>
+        <v>1323740</v>
       </c>
       <c r="C44" s="4">
-        <v>28168200000</v>
+        <v>61829437</v>
       </c>
       <c r="D44" s="3">
-        <v>24848980000</v>
+        <v>2839096</v>
       </c>
       <c r="E44" s="3">
-        <v>1321649000</v>
+        <v>1832250</v>
       </c>
       <c r="F44" s="3">
         <v>2209</v>
@@ -5607,16 +5559,16 @@
         <v>2048</v>
       </c>
       <c r="B45" s="4">
-        <v>988585000</v>
+        <v>1356027</v>
       </c>
       <c r="C45" s="4">
-        <v>52811757743</v>
+        <v>127336866</v>
       </c>
       <c r="D45" s="3">
-        <v>48093805000</v>
+        <v>3248070</v>
       </c>
       <c r="E45" s="3">
-        <v>1218420000</v>
+        <v>1870407</v>
       </c>
       <c r="F45" s="3">
         <v>4356</v>
@@ -5628,16 +5580,16 @@
         <v>4096</v>
       </c>
       <c r="B46" s="4">
-        <v>914418000</v>
+        <v>1369963</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D46" s="3">
-        <v>145792731000</v>
+        <v>4402775</v>
       </c>
       <c r="E46" s="3">
-        <v>1331453000</v>
+        <v>1729132</v>
       </c>
       <c r="F46" s="3">
         <v>8649</v>
@@ -5649,16 +5601,16 @@
         <v>8192</v>
       </c>
       <c r="B47" s="4">
-        <v>3169282000</v>
+        <v>1781902</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D47" s="3">
-        <v>290431819000</v>
+        <v>6615509</v>
       </c>
       <c r="E47" s="3">
-        <v>1427040000</v>
+        <v>1883162</v>
       </c>
       <c r="F47" s="3">
         <v>17424</v>
@@ -5670,29 +5622,62 @@
         <v>16384</v>
       </c>
       <c r="B48" s="4">
-        <v>31489207000</v>
+        <v>49863209</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>5</v>
+      <c r="D48" s="3">
+        <v>12836717</v>
       </c>
       <c r="E48" s="3">
-        <v>1458768000</v>
+        <v>1974957</v>
       </c>
       <c r="F48" s="3">
         <v>34969</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="4"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="4"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="4"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="4"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="4"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="4"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="4"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="4"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="4"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="4"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="4"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B64" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B65" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -5721,13 +5706,13 @@
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="4">
-        <v>722000</v>
+        <v>777</v>
       </c>
       <c r="D67" s="3">
-        <v>103183000</v>
+        <v>507881</v>
       </c>
       <c r="E67" s="3">
-        <v>1519057000</v>
+        <v>508680</v>
       </c>
       <c r="F67" s="3">
         <v>4</v>
@@ -5739,16 +5724,16 @@
         <v>4</v>
       </c>
       <c r="B68" s="4">
-        <v>305209000</v>
+        <v>507057</v>
       </c>
       <c r="C68" s="4">
-        <v>203249000</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>10</v>
+        <v>203687</v>
+      </c>
+      <c r="D68" s="3">
+        <v>509705</v>
       </c>
       <c r="E68" s="3">
-        <v>818390000</v>
+        <v>1114825</v>
       </c>
       <c r="F68" s="3">
         <v>9</v>
@@ -5760,16 +5745,16 @@
         <v>8</v>
       </c>
       <c r="B69" s="4">
-        <v>405576000</v>
+        <v>507972</v>
       </c>
       <c r="C69" s="4">
-        <v>820825000</v>
+        <v>205375</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E69" s="3">
-        <v>1244022000</v>
+        <v>2133553</v>
       </c>
       <c r="F69" s="3">
         <v>16</v>
@@ -5781,16 +5766,16 @@
         <v>16</v>
       </c>
       <c r="B70" s="4">
-        <v>512705000</v>
+        <v>512343</v>
       </c>
       <c r="C70" s="4">
-        <v>1024733000</v>
+        <v>510074</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E70" s="3">
-        <v>2392942000</v>
+        <v>2566066</v>
       </c>
       <c r="F70" s="3">
         <v>36</v>
@@ -5802,16 +5787,13 @@
         <v>32</v>
       </c>
       <c r="B71" s="4">
-        <v>519475000</v>
+        <v>1425194</v>
       </c>
       <c r="C71" s="4">
-        <v>2926346000</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>5</v>
+        <v>317462</v>
       </c>
       <c r="E71" s="3">
-        <v>2086793000</v>
+        <v>1577064</v>
       </c>
       <c r="F71" s="3">
         <v>64</v>
@@ -5823,16 +5805,13 @@
         <v>64</v>
       </c>
       <c r="B72" s="4">
-        <v>753616000</v>
+        <v>1139205</v>
       </c>
       <c r="C72" s="4">
-        <v>3872559000</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>5</v>
+        <v>433415</v>
       </c>
       <c r="E72" s="3">
-        <v>2890661000</v>
+        <v>4003734</v>
       </c>
       <c r="F72" s="3">
         <v>121</v>
@@ -5844,16 +5823,16 @@
         <v>128</v>
       </c>
       <c r="B73" s="4">
-        <v>889608000</v>
+        <v>1089458</v>
       </c>
       <c r="C73" s="4">
-        <v>3496309000</v>
+        <v>691443</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E73" s="3">
-        <v>5470549000</v>
+        <v>4823738</v>
       </c>
       <c r="F73" s="3">
         <v>256</v>
@@ -5865,16 +5844,16 @@
         <v>256</v>
       </c>
       <c r="B74" s="4">
-        <v>1014064000</v>
+        <v>1514786</v>
       </c>
       <c r="C74" s="4">
-        <v>3840595000</v>
+        <v>808164</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E74" s="3">
-        <v>6261039000</v>
+        <v>5620980</v>
       </c>
       <c r="F74" s="3">
         <v>529</v>
@@ -5886,16 +5865,16 @@
         <v>512</v>
       </c>
       <c r="B75" s="4">
-        <v>1244979000</v>
+        <v>2017870</v>
       </c>
       <c r="C75" s="4">
-        <v>4301601000</v>
+        <v>1068686</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E75" s="3">
-        <v>7489979000</v>
+        <v>8556942</v>
       </c>
       <c r="F75" s="3">
         <v>1089</v>
@@ -5907,16 +5886,16 @@
         <v>1024</v>
       </c>
       <c r="B76" s="4">
-        <v>1761898000</v>
+        <v>2462571</v>
       </c>
       <c r="C76" s="4">
-        <v>5887163000</v>
+        <v>1641384</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E76" s="3">
-        <v>9205334000</v>
+        <v>8617073</v>
       </c>
       <c r="F76" s="3">
         <v>2209</v>
@@ -5928,16 +5907,16 @@
         <v>2048</v>
       </c>
       <c r="B77" s="4">
-        <v>5423181000</v>
+        <v>5940121</v>
       </c>
       <c r="C77" s="4">
-        <v>7266657000</v>
+        <v>5982439</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E77" s="3">
-        <v>21032582000</v>
+        <v>10408258</v>
       </c>
       <c r="F77" s="3">
         <v>4356</v>
@@ -5949,16 +5928,16 @@
         <v>4096</v>
       </c>
       <c r="B78" s="4">
-        <v>12085779000</v>
+        <v>16119075</v>
       </c>
       <c r="C78" s="4">
-        <v>10008529000</v>
+        <v>18976081</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E78" s="3">
-        <v>46976933000</v>
+        <v>24651993</v>
       </c>
       <c r="F78" s="3">
         <v>8649</v>
@@ -5970,16 +5949,16 @@
         <v>8192</v>
       </c>
       <c r="B79" s="4">
-        <v>62770179000</v>
+        <v>69764083</v>
       </c>
       <c r="C79" s="4">
-        <v>15759075000</v>
+        <v>65690642</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E79" s="3" t="s">
-        <v>5</v>
+      <c r="E79" s="3">
+        <v>47924722</v>
       </c>
       <c r="F79" s="3">
         <v>17424</v>
@@ -5993,8 +5972,8 @@
       <c r="B80" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C80" s="4">
-        <v>27411723000</v>
+      <c r="C80" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>5</v>
@@ -6005,6 +5984,45 @@
       <c r="F80" s="3">
         <v>34969</v>
       </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="4"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="4"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="4"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="4"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="4"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="4"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="4"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="4"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="4"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="4"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="4"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B94" s="1"/>

</xml_diff>

<commit_message>
Cleanup + changed README
</commit_message>
<xml_diff>
--- a/Graphs.xlsx
+++ b/Graphs.xlsx
@@ -696,7 +696,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="diamond"/>
+            <c:symbol val="square"/>
             <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
@@ -4964,8 +4964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Removed debug statements. Changed README
</commit_message>
<xml_diff>
--- a/Graphs.xlsx
+++ b/Graphs.xlsx
@@ -1388,133 +1388,8 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>Line</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$35:$A$48</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>256.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1024.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2048.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4096.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8192.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>16384.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$35:$C$45</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>813138.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>812748.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>913472.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.621754E6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.327589E6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.026578E6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9.196144E6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.398393E6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.1228694E7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6.1829437E7</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.27336866E8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
           <c:tx>
             <c:v>2D</c:v>
           </c:tx>
@@ -1642,7 +1517,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>imp2D</c:v>
           </c:tx>
@@ -1768,6 +1643,122 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1.974957E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Line</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$35:$A$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$35:$C$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>813138.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>812748.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>913472.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.621754E6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.327589E6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.026578E6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.196144E6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.398393E6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.1228694E7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.1829437E7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.27336866E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4964,8 +4955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Change readme to reflect problems with pushsum + 2D
</commit_message>
<xml_diff>
--- a/Graphs.xlsx
+++ b/Graphs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paanir/Distributed-Systems-Projects/project2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paanir/Distributed-Systems-Projects/Proj2/project2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -194,7 +194,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1400"/>
               <a:t>Graph-1</a:t>
             </a:r>
           </a:p>
@@ -203,11 +203,11 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1400"/>
               <a:t>Convergence times for gossip</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
               <a:t> </a:t>
             </a:r>
           </a:p>
@@ -216,7 +216,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
               <a:t>(where convergence means all nodes have heard the rumor at least once)</a:t>
             </a:r>
           </a:p>
@@ -811,11 +811,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1054790192"/>
-        <c:axId val="-1054785648"/>
+        <c:axId val="-1051106880"/>
+        <c:axId val="-1050960608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1054790192"/>
+        <c:axId val="-1051106880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -928,12 +928,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1054785648"/>
+        <c:crossAx val="-1050960608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1054785648"/>
+        <c:axId val="-1050960608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1047,7 +1047,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1054790192"/>
+        <c:crossAx val="-1051106880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1773,11 +1773,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1054754752"/>
-        <c:axId val="-1054750480"/>
+        <c:axId val="-1098170176"/>
+        <c:axId val="-1098212640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1054754752"/>
+        <c:axId val="-1098170176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1858,6 +1858,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1894,12 +1895,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1054750480"/>
+        <c:crossAx val="-1098212640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1054750480"/>
+        <c:axId val="-1098212640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2016,7 +2017,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1054754752"/>
+        <c:crossAx val="-1098170176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2589,11 +2590,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1054718688"/>
-        <c:axId val="-1054714928"/>
+        <c:axId val="-1016236752"/>
+        <c:axId val="-1016233632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1054718688"/>
+        <c:axId val="-1016236752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2710,12 +2711,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1054714928"/>
+        <c:crossAx val="-1016233632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1054714928"/>
+        <c:axId val="-1016233632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2833,7 +2834,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1054718688"/>
+        <c:crossAx val="-1016236752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4955,8 +4956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Changed readme and project.ex to create separate graphs for pushsum + 2d and pushsum + line. for 2d, threshold changed to 1 rather than 75%
</commit_message>
<xml_diff>
--- a/Graphs.xlsx
+++ b/Graphs.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
   <si>
     <t>num_nodes</t>
   </si>
@@ -54,22 +54,46 @@
     <t>Convergence = All nodes have heard the rumor at least once</t>
   </si>
   <si>
-    <t>line (50%)</t>
+    <t>Convergence times for Push-Sum + 2D</t>
   </si>
   <si>
-    <t>Convergence = 75 % of nodes have converged to some value (50% for line topology)</t>
+    <t>Convergence = At least one node gets the correct value of global average</t>
   </si>
   <si>
-    <t>Consider it to be the y-axis</t>
+    <t>Convergence for Push-Sum + Line</t>
   </si>
   <si>
-    <t>Convergence times for Gossip (in microseconds)</t>
+    <t>Convergence = 50% of nodes have converged to some value (not necessarily global average)</t>
   </si>
   <si>
-    <t>Convergence times for Push-Sum (in microseconds)</t>
+    <t>Graph-1-1</t>
   </si>
   <si>
-    <t>Converge very slowly</t>
+    <t>Graph-1-2</t>
+  </si>
+  <si>
+    <t>Graph-2-1</t>
+  </si>
+  <si>
+    <t>Graph-2-2</t>
+  </si>
+  <si>
+    <t>Graph-2-3</t>
+  </si>
+  <si>
+    <t>Convergence times for Push-Sum + Full and Push-Sum + imp2D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convergence times for Gossip </t>
+  </si>
+  <si>
+    <t>Convergence times for Gossip</t>
+  </si>
+  <si>
+    <t>Convergence = 75 % of nodes have converged to the global average</t>
+  </si>
+  <si>
+    <t>Line</t>
   </si>
 </sst>
 </file>
@@ -195,7 +219,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1400"/>
-              <a:t>Graph-1</a:t>
+              <a:t>Graph-1-1</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -811,11 +835,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1051106880"/>
-        <c:axId val="-1050960608"/>
+        <c:axId val="-1054921104"/>
+        <c:axId val="-1054917888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1051106880"/>
+        <c:axId val="-1054921104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -928,12 +952,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1050960608"/>
+        <c:crossAx val="-1054917888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1050960608"/>
+        <c:axId val="-1054917888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1047,7 +1071,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1051106880"/>
+        <c:crossAx val="-1054921104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1174,7 +1198,7 @@
               <a:rPr lang="en-US" sz="1400" b="1" i="0" cap="all" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Graph-2</a:t>
+              <a:t>Graph-1-2</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -1207,7 +1231,14 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.19730509173564"/>
+          <c:y val="0.0216919739696312"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1773,11 +1804,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1098170176"/>
-        <c:axId val="-1098212640"/>
+        <c:axId val="-1019397136"/>
+        <c:axId val="-1019393504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1098170176"/>
+        <c:axId val="-1019397136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1895,12 +1926,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1098212640"/>
+        <c:crossAx val="-1019393504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1098212640"/>
+        <c:axId val="-1019393504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2017,7 +2048,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1098170176"/>
+        <c:crossAx val="-1019397136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2142,7 +2173,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Graph-3</a:t>
+              <a:t>Graph-2-1</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -2151,11 +2182,16 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Convergence times for Push-Sum</a:t>
+              <a:t>Convergence times for Push-Sum + Full and Push-Sum + imp2D</a:t>
             </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> (Where Convergence mean 75% of nodes converged to a value)</a:t>
+              <a:t>Convergence is defined as 75% of nodes converge to the global average  </a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2412,48 +2448,12 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$67:$C$79</c:f>
+              <c:f>Sheet1!#REF!</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>777.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>203687.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>205375.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>510074.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>317462.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>433415.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>691443.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>808164.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.068686E6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.641384E6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5.982439E6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.8976081E7</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6.5690642E7</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2492,7 +2492,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$67:$F$78</c:f>
+              <c:f>Sheet1!$D$67:$D$78</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2537,7 +2537,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$67:$E$78</c:f>
+              <c:f>Sheet1!$C$67:$C$78</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2590,11 +2590,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1016236752"/>
-        <c:axId val="-1016233632"/>
+        <c:axId val="-1055139248"/>
+        <c:axId val="-1055136128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1016236752"/>
+        <c:axId val="-1055139248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2711,12 +2711,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1016233632"/>
+        <c:crossAx val="-1055136128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1016233632"/>
+        <c:axId val="-1055136128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2834,7 +2834,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1016236752"/>
+        <c:crossAx val="-1055139248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2848,6 +2848,10 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
@@ -2920,6 +2924,1089 @@
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="is-IS"/>
+              <a:t>Graph 2-2</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="is-IS"/>
+              <a:t>Convergence times for Push-Sum + 2D</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="is-IS"/>
+              <a:t>Where convergence is defined as at least</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="is-IS" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="is-IS"/>
+              <a:t>one node converging to the</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="is-IS" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="is-IS"/>
+              <a:t>global average</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.109755880029559"/>
+          <c:y val="0.171622418879056"/>
+          <c:w val="0.850761919323192"/>
+          <c:h val="0.720123104081016"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>2D</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$95:$A$107</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>121.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>529.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1089.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2209.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4356.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8649.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17424.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$95:$B$107</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>5661.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12575.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30471.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120611.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>399888.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.222203E6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.845723E6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.354392E6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.040381E6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.28213E6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>207144.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>423826.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>388155.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1049036624"/>
+        <c:axId val="-1098576512"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1049036624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of nodes in topology</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1098576512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1098576512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Times in Microseconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1049036624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Graph 2-3</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Convergence times for Push-Sum + Line</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Where convergence is defined as 50% of nodes converging to some value</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.115272076791618"/>
+          <c:y val="0.109418181818182"/>
+          <c:w val="0.850001756879781"/>
+          <c:h val="0.764406299212598"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Line</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$118:$A$130</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$118:$B$130</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>777.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>203687.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>205375.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>510074.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>317462.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>433415.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>691443.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>808164.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.068686E6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.641384E6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.982439E6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.8976081E7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.5690642E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1015562000"/>
+        <c:axId val="-1019480192"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1015562000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of nodes in topology</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1019480192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1019480192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Times</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> in</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t> microseconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1015562000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -3044,6 +4131,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
   <cs:axisTitle>
@@ -4081,6 +5248,1038 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4660,16 +6859,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
       <xdr:row>87</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4683,6 +6882,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4954,10 +7213,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F110"/>
+  <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4973,8 +7232,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -5307,8 +7569,11 @@
       <c r="C21" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B32" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -5663,16 +7928,19 @@
       <c r="A59" s="4"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B64" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B65" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>0</v>
       </c>
@@ -5680,37 +7948,25 @@
         <v>1</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F66" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>2</v>
       </c>
       <c r="B67" s="4"/>
-      <c r="C67" s="4">
-        <v>777</v>
+      <c r="C67" s="3">
+        <v>508680</v>
       </c>
       <c r="D67" s="3">
-        <v>507881</v>
-      </c>
-      <c r="E67" s="3">
-        <v>508680</v>
-      </c>
-      <c r="F67" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <f>2 *A67</f>
         <v>4</v>
@@ -5718,20 +7974,14 @@
       <c r="B68" s="4">
         <v>507057</v>
       </c>
-      <c r="C68" s="4">
-        <v>203687</v>
+      <c r="C68" s="3">
+        <v>1114825</v>
       </c>
       <c r="D68" s="3">
-        <v>509705</v>
-      </c>
-      <c r="E68" s="3">
-        <v>1114825</v>
-      </c>
-      <c r="F68" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <f t="shared" ref="A69:A80" si="2">2 *A68</f>
         <v>8</v>
@@ -5739,20 +7989,14 @@
       <c r="B69" s="4">
         <v>507972</v>
       </c>
-      <c r="C69" s="4">
-        <v>205375</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E69" s="3">
+      <c r="C69" s="3">
         <v>2133553</v>
       </c>
-      <c r="F69" s="3">
+      <c r="D69" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -5760,20 +8004,14 @@
       <c r="B70" s="4">
         <v>512343</v>
       </c>
-      <c r="C70" s="4">
-        <v>510074</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E70" s="3">
+      <c r="C70" s="3">
         <v>2566066</v>
       </c>
-      <c r="F70" s="3">
+      <c r="D70" s="3">
         <v>36</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -5781,17 +8019,14 @@
       <c r="B71" s="4">
         <v>1425194</v>
       </c>
-      <c r="C71" s="4">
-        <v>317462</v>
-      </c>
-      <c r="E71" s="3">
+      <c r="C71" s="3">
         <v>1577064</v>
       </c>
-      <c r="F71" s="3">
+      <c r="D71" s="3">
         <v>64</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <f t="shared" si="2"/>
         <v>64</v>
@@ -5799,17 +8034,14 @@
       <c r="B72" s="4">
         <v>1139205</v>
       </c>
-      <c r="C72" s="4">
-        <v>433415</v>
-      </c>
-      <c r="E72" s="3">
+      <c r="C72" s="3">
         <v>4003734</v>
       </c>
-      <c r="F72" s="3">
+      <c r="D72" s="3">
         <v>121</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
         <f t="shared" si="2"/>
         <v>128</v>
@@ -5817,20 +8049,14 @@
       <c r="B73" s="4">
         <v>1089458</v>
       </c>
-      <c r="C73" s="4">
-        <v>691443</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E73" s="3">
+      <c r="C73" s="3">
         <v>4823738</v>
       </c>
-      <c r="F73" s="3">
+      <c r="D73" s="3">
         <v>256</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
         <f t="shared" si="2"/>
         <v>256</v>
@@ -5838,20 +8064,14 @@
       <c r="B74" s="4">
         <v>1514786</v>
       </c>
-      <c r="C74" s="4">
-        <v>808164</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E74" s="3">
+      <c r="C74" s="3">
         <v>5620980</v>
       </c>
-      <c r="F74" s="3">
+      <c r="D74" s="3">
         <v>529</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
         <f t="shared" si="2"/>
         <v>512</v>
@@ -5859,20 +8079,14 @@
       <c r="B75" s="4">
         <v>2017870</v>
       </c>
-      <c r="C75" s="4">
-        <v>1068686</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E75" s="3">
+      <c r="C75" s="3">
         <v>8556942</v>
       </c>
-      <c r="F75" s="3">
+      <c r="D75" s="3">
         <v>1089</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
         <f t="shared" si="2"/>
         <v>1024</v>
@@ -5880,20 +8094,14 @@
       <c r="B76" s="4">
         <v>2462571</v>
       </c>
-      <c r="C76" s="4">
-        <v>1641384</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E76" s="3">
+      <c r="C76" s="3">
         <v>8617073</v>
       </c>
-      <c r="F76" s="3">
+      <c r="D76" s="3">
         <v>2209</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
         <f t="shared" si="2"/>
         <v>2048</v>
@@ -5901,20 +8109,14 @@
       <c r="B77" s="4">
         <v>5940121</v>
       </c>
-      <c r="C77" s="4">
-        <v>5982439</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E77" s="3">
+      <c r="C77" s="3">
         <v>10408258</v>
       </c>
-      <c r="F77" s="3">
+      <c r="D77" s="3">
         <v>4356</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
         <f t="shared" si="2"/>
         <v>4096</v>
@@ -5922,20 +8124,14 @@
       <c r="B78" s="4">
         <v>16119075</v>
       </c>
-      <c r="C78" s="4">
-        <v>18976081</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E78" s="3">
+      <c r="C78" s="3">
         <v>24651993</v>
       </c>
-      <c r="F78" s="3">
+      <c r="D78" s="3">
         <v>8649</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
         <f t="shared" si="2"/>
         <v>8192</v>
@@ -5943,20 +8139,14 @@
       <c r="B79" s="4">
         <v>69764083</v>
       </c>
-      <c r="C79" s="4">
-        <v>65690642</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E79" s="3">
+      <c r="C79" s="3">
         <v>47924722</v>
       </c>
-      <c r="F79" s="3">
+      <c r="D79" s="3">
         <v>17424</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
         <f t="shared" si="2"/>
         <v>16384</v>
@@ -5964,16 +8154,10 @@
       <c r="B80" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C80" s="4" t="s">
+      <c r="C80" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D80" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F80" s="3">
+      <c r="D80" s="3">
         <v>34969</v>
       </c>
     </row>
@@ -6016,111 +8200,186 @@
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="4"/>
     </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B93" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B94" s="1"/>
+      <c r="A94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B95" s="1"/>
+      <c r="A95" s="3">
+        <v>4</v>
+      </c>
+      <c r="B95" s="3">
+        <v>5661</v>
+      </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
+      <c r="A96" s="3">
+        <v>9</v>
+      </c>
+      <c r="B96" s="3">
+        <v>12575</v>
+      </c>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" s="4"/>
-      <c r="B97" s="4"/>
+      <c r="A97" s="3">
+        <v>16</v>
+      </c>
+      <c r="B97" s="3">
+        <v>30471</v>
+      </c>
       <c r="C97" s="4"/>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A98" s="4"/>
-      <c r="B98" s="4"/>
+      <c r="A98" s="3">
+        <v>36</v>
+      </c>
+      <c r="B98" s="3">
+        <v>120611</v>
+      </c>
       <c r="C98" s="4"/>
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99" s="4"/>
-      <c r="B99" s="4"/>
+      <c r="A99" s="3">
+        <v>64</v>
+      </c>
+      <c r="B99" s="3">
+        <v>399888</v>
+      </c>
       <c r="C99" s="4"/>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100" s="4"/>
-      <c r="B100" s="4"/>
+      <c r="A100" s="3">
+        <v>121</v>
+      </c>
+      <c r="B100" s="3">
+        <v>1222203</v>
+      </c>
       <c r="C100" s="4"/>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" s="4"/>
-      <c r="B101" s="4"/>
+      <c r="A101" s="3">
+        <v>256</v>
+      </c>
+      <c r="B101" s="3">
+        <v>6845723</v>
+      </c>
       <c r="C101" s="4"/>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102" s="4"/>
-      <c r="B102" s="4"/>
+      <c r="A102" s="3">
+        <v>529</v>
+      </c>
+      <c r="B102" s="3">
+        <v>9354392</v>
+      </c>
       <c r="C102" s="4"/>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103" s="4"/>
-      <c r="B103" s="4"/>
+      <c r="A103" s="3">
+        <v>1089</v>
+      </c>
+      <c r="B103" s="3">
+        <v>6040381</v>
+      </c>
       <c r="C103" s="4"/>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>
       <c r="F103" s="3"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A104" s="4"/>
-      <c r="B104" s="4"/>
+      <c r="A104" s="3">
+        <v>2209</v>
+      </c>
+      <c r="B104" s="3">
+        <v>2282130</v>
+      </c>
       <c r="C104" s="4"/>
       <c r="D104" s="3"/>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A105" s="4"/>
-      <c r="B105" s="4"/>
+      <c r="A105" s="3">
+        <v>4356</v>
+      </c>
+      <c r="B105" s="3">
+        <v>207144</v>
+      </c>
       <c r="C105" s="4"/>
       <c r="D105" s="3"/>
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A106" s="4"/>
-      <c r="B106" s="4"/>
+      <c r="A106" s="3">
+        <v>8649</v>
+      </c>
+      <c r="B106" s="3">
+        <v>423826</v>
+      </c>
       <c r="C106" s="4"/>
       <c r="D106" s="3"/>
       <c r="E106" s="3"/>
       <c r="F106" s="3"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A107" s="4"/>
-      <c r="B107" s="4"/>
+      <c r="A107" s="3">
+        <v>17424</v>
+      </c>
+      <c r="B107" s="3">
+        <v>388155</v>
+      </c>
       <c r="C107" s="4"/>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A108" s="4"/>
-      <c r="B108" s="4"/>
+      <c r="A108" s="3">
+        <v>34969</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C108" s="4"/>
       <c r="D108" s="3"/>
       <c r="E108" s="3"/>
@@ -6141,6 +8400,152 @@
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B116" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="4">
+        <v>2</v>
+      </c>
+      <c r="B118" s="4">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="4">
+        <f>2 *A118</f>
+        <v>4</v>
+      </c>
+      <c r="B119" s="4">
+        <v>203687</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="4">
+        <f t="shared" ref="A120:A131" si="3">2 *A119</f>
+        <v>8</v>
+      </c>
+      <c r="B120" s="4">
+        <v>205375</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="4">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="B121" s="4">
+        <v>510074</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="4">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="B122" s="4">
+        <v>317462</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="4">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="B123" s="4">
+        <v>433415</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="4">
+        <f t="shared" si="3"/>
+        <v>128</v>
+      </c>
+      <c r="B124" s="4">
+        <v>691443</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="4">
+        <f t="shared" si="3"/>
+        <v>256</v>
+      </c>
+      <c r="B125" s="4">
+        <v>808164</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="4">
+        <f t="shared" si="3"/>
+        <v>512</v>
+      </c>
+      <c r="B126" s="4">
+        <v>1068686</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="4">
+        <f t="shared" si="3"/>
+        <v>1024</v>
+      </c>
+      <c r="B127" s="4">
+        <v>1641384</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="4">
+        <f t="shared" si="3"/>
+        <v>2048</v>
+      </c>
+      <c r="B128" s="4">
+        <v>5982439</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="4">
+        <f t="shared" si="3"/>
+        <v>4096</v>
+      </c>
+      <c r="B129" s="4">
+        <v>18976081</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="4">
+        <f t="shared" si="3"/>
+        <v>8192</v>
+      </c>
+      <c r="B130" s="4">
+        <v>65690642</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="4">
+        <f t="shared" si="3"/>
+        <v>16384</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>